<commit_message>
Entregando a prova rev1
</commit_message>
<xml_diff>
--- a/T2C/Output/Relatorio.xlsx
+++ b/T2C/Output/Relatorio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://t2cconsultoria365-my.sharepoint.com/personal/maycon_rosa_t2cgroup_com_br/Documents/Documentos/UiPath/prj_Prova_PraticaUipath/T2C/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{CBD3AE35-E206-4D12-B5DA-8D2B82C2223D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7322413F-3316-4D31-9B60-92EB5045AF77}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="8_{CBD3AE35-E206-4D12-B5DA-8D2B82C2223D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3402103-68D7-4308-AB39-B37AFC88A0F7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EA7588BA-F026-4AAF-9BDA-D450FBE1DB3C}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{EA7588BA-F026-4AAF-9BDA-D450FBE1DB3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Piores" sheetId="2" r:id="rId1"/>
@@ -37,12 +37,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Nome do Produto</t>
   </si>
   <si>
     <t>Qtd Estrelas</t>
+  </si>
+  <si>
+    <t>Maneater - PS4</t>
+  </si>
+  <si>
+    <t>Jogo PS4 - God of War - Playstation Hits - Playstation</t>
+  </si>
+  <si>
+    <t>Jogo Ps4 Scarlet Nexus Game</t>
+  </si>
+  <si>
+    <t>Suporte Ps4 Slim Horizontal Pezinho Elevação Altura Laranja</t>
+  </si>
+  <si>
+    <t>Controle Para Ps4 Sem Fio Double Motor Vibration 4</t>
+  </si>
+  <si>
+    <t>Jogo Nioh - PS4</t>
+  </si>
+  <si>
+    <t>Lego Worlds - Ps4</t>
+  </si>
+  <si>
+    <t>Battlefield V 5 PS4</t>
+  </si>
+  <si>
+    <t>Jogo Pes 2021 - Ps4</t>
+  </si>
+  <si>
+    <t>Jogo Oddworld Soulstorm - PS4</t>
+  </si>
+  <si>
+    <t>Jogo Resident Evil 3 - PS4</t>
+  </si>
+  <si>
+    <t>Ps4 - Terra-Média: Sombras Da Guerra Definitive Edition</t>
+  </si>
+  <si>
+    <t>The Crew 2 - Ps4</t>
+  </si>
+  <si>
+    <t>Mortal Kombat X - Ps4</t>
+  </si>
+  <si>
+    <t>Jogo Mad Max - Ps4</t>
+  </si>
+  <si>
+    <t>Jogo Pacman Museum + PS4</t>
+  </si>
+  <si>
+    <t>Jogo Hitman 2 - PS4</t>
+  </si>
+  <si>
+    <t>Jogo Cyberpunk 2077 - Ps4</t>
+  </si>
+  <si>
+    <t>Ratchet E Clank Hits - PS4</t>
+  </si>
+  <si>
+    <t>Jogo Resident Evil 3 Remake - Ps4</t>
   </si>
 </sst>
 </file>
@@ -398,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8B7584-AE09-4D22-9C5E-1CB7D70BAB6B}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -416,6 +476,166 @@
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>